<commit_message>
added some of Luis's pubs
</commit_message>
<xml_diff>
--- a/Prep/Pubs_Import.xlsx
+++ b/Prep/Pubs_Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamilton/Documents/WIP/ready4/Code/Brochure/HTML/nmhsmn_web/Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D8E53C-EA3D-A342-A28C-FAE91554BDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CDEEFC-A378-EB44-A6E2-539FAA611918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="4500" windowWidth="33280" windowHeight="17440" xr2:uid="{313AAF49-2FE8-0C4B-87F0-D1663512E606}"/>
+    <workbookView xWindow="22080" yWindow="16860" windowWidth="33280" windowHeight="17440" xr2:uid="{313AAF49-2FE8-0C4B-87F0-D1663512E606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>First Author</t>
   </si>
@@ -103,13 +103,58 @@
   </si>
   <si>
     <t>There is a strong case for inclusion of systems modelling in the analytic tool kit for identifying targeted investments likely to deliver efficient, effective &amp; equitable impacts.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.ijinfomgt.2019.04.012</t>
+  </si>
+  <si>
+    <t>Younjin Chung</t>
+  </si>
+  <si>
+    <t>Scoping review.</t>
+  </si>
+  <si>
+    <t>Visual analytics is needed for mental healthcare systems research and policy.</t>
+  </si>
+  <si>
+    <t>Data Visualisation, Regional Planning, Uses of Modelling</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0212179</t>
+  </si>
+  <si>
+    <t>Carlos R. García-Alonso</t>
+  </si>
+  <si>
+    <t>A Monte-Carlo simulation combined with a fuzzy inference engine was used to examine the Relative Technical Efficiency (RTE) of three proposed intervention scenarios.</t>
+  </si>
+  <si>
+    <t>Decision makers can use information from this approach to design new interventions and policies.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpsyt.2023.993197</t>
+  </si>
+  <si>
+    <t>Jose A. Salinas-Perez</t>
+  </si>
+  <si>
+    <t>Mental health services in three countries were described and classified using the Description and Evaluation of Services and Directories of Long Term Care mapping tool.</t>
+  </si>
+  <si>
+    <t>Data on mental health provision in rural areas should be gathered using standardized methods and used to inform rural service planning.</t>
+  </si>
+  <si>
+    <t>Rural Mental Health, Taxonomies</t>
+  </si>
+  <si>
+    <t>Model Implementation, Regional Planning, Technical Efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +210,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF606060"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -196,6 +247,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F5063A-17F0-3B42-83B6-1158BD3A3BE6}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,9 +723,87 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{3554CFCF-D4A8-B44F-AA47-89E52DF2022E}"/>
+    <hyperlink ref="A6" r:id="rId2" tooltip="Persistent link using digital object identifier" xr:uid="{E0103561-65EC-9C4F-85BF-EB3C9352A0FE}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{456DB74F-EAA2-C947-82DB-5CD76A5D2A4D}"/>
+    <hyperlink ref="A8" r:id="rId4" xr:uid="{51F02C89-ABD4-564D-A031-AD2B8F377266}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>